<commit_message>
Alterações de layout e finalização da modelagem do BD
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Expandir</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t>Testar Modelos e BD</t>
   </si>
@@ -184,16 +178,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -218,7 +206,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +240,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,18 +321,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -350,25 +341,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,221 +444,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>2447925</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Button 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Reduzir</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>2447925</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>2428875</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Normal</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>2438400</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Button 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Aumentar</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -926,14 +708,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -943,18 +725,11 @@
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
+    <row r="1" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
       <c r="B4" s="4">
         <v>42373</v>
       </c>
@@ -975,72 +750,74 @@
         <v>42377</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="9" t="s">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="E7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
       <c r="B10" s="4">
         <f>F4+3</f>
         <v>42380</v>
@@ -1062,69 +839,69 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="9" t="s">
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <f>F10+3</f>
         <v>42387</v>
@@ -1146,75 +923,75 @@
         <v>42391</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="9" t="s">
+    <row r="18" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="D20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
         <f>F17+3</f>
         <v>42394</v>
@@ -1236,74 +1013,74 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="9" t="s">
+    <row r="25" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>50</v>
+      <c r="D25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="9" t="s">
-        <v>45</v>
+    <row r="27" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="9" t="s">
-        <v>47</v>
+    <row r="28" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="2:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1534,80 +1311,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Reduzir">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>2447925</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Button 2">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Normal">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>2447925</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>2428875</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId6" name="Button 3">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Aumentar">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>2438400</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -1636,749 +1339,749 @@
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>16</v>
+      <c r="B2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <f t="shared" ref="A3" si="0">IF(C3 &lt;&gt; 0,A2+1)</f>
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="6">
         <f>IF(C3&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="str">
+      <c r="E3" s="8" t="str">
         <f>IF(C3&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>17</v>
+      <c r="H3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <f>IF(C5 &lt;&gt; 0,A3+1)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6">
         <f>IF(C5&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>18</v>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <f>IF(C7 &lt;&gt; 0,A4+1)</f>
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ref="D5:D10" si="1">IF(C7&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="str">
+      <c r="E5" s="8" t="str">
         <f t="shared" ref="E5:E12" si="2">IF(C7&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <f>IF(C8 &lt;&gt; 0,A5+1)</f>
         <v>4</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E6" s="9" t="str">
+      <c r="E6" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <f>IF(C9 &lt;&gt; 0,A6+1)</f>
         <v>5</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E7" s="9" t="str">
+      <c r="E7" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <f>IF(C10 &lt;&gt; 0,A7+1)</f>
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E8" s="9" t="str">
+      <c r="E8" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <f>IF(C11 &lt;&gt; 0,A8+1)</f>
         <v>7</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E9" s="9" t="str">
+      <c r="E9" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <f>IF(C12 &lt;&gt; 0,A9+1,"")</f>
         <v>8</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E10" s="9" t="str">
+      <c r="E10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17">
+      <c r="A11" s="16">
         <f>IF(C13 &lt;&gt; 0,A10+1,"")</f>
         <v>9</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
       </c>
-      <c r="E11" s="9" t="str">
+      <c r="E11" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <f>IF(C14 &lt;&gt; 0,A11+1,"")</f>
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="6">
         <f>IF(C14&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E12" s="9" t="str">
+      <c r="E12" s="8" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17">
+      <c r="A13" s="16">
         <f t="shared" ref="A13:A23" si="3">IF(C14 &lt;&gt; 0,A12+1,"")</f>
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" ref="D13:D23" si="4">IF(C14&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E13" s="9" t="str">
+      <c r="E13" s="8" t="str">
         <f t="shared" ref="E13:E23" si="5">IF(C14&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E14" s="9" t="str">
+      <c r="E14" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E15" s="9" t="str">
+      <c r="E15" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E16" s="9" t="str">
+      <c r="E16" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
+      <c r="A17" s="16">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E17" s="9" t="str">
+      <c r="E17" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E18" s="9" t="str">
+      <c r="E18" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E19" s="9" t="str">
+      <c r="E19" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E20" s="9" t="str">
+      <c r="E20" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17">
+      <c r="A21" s="16">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E21" s="9" t="str">
+      <c r="E21" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E22" s="9" t="str">
+      <c r="E22" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17">
+      <c r="A23" s="16">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E23" s="9" t="str">
+      <c r="E23" s="8" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <f>IF(C24&lt;&gt; 0,A23+1,"")</f>
         <v>22</v>
       </c>
-      <c r="B24" s="15"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" s="6">
         <f>IF(C24&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E24" s="9" t="str">
+      <c r="E24" s="8" t="str">
         <f>IF(C24&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17">
+      <c r="A25" s="16">
         <f>IF(C25 &lt;&gt; 0,A24+1,"")</f>
         <v>23</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D25" s="6">
         <f>IF(C25&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E25" s="9" t="str">
+      <c r="E25" s="8" t="str">
         <f>IF(C25&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <f t="shared" ref="A26" si="6">IF(C26 &lt;&gt; 0,A25+1,"")</f>
         <v>24</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26" si="7">IF(C26&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="8" t="str">
         <f t="shared" ref="E26" si="8">IF(C26&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17">
+      <c r="A27" s="16">
         <f t="shared" ref="A27:A73" si="9">IF(C27 &lt;&gt; 0,A26+1,"")</f>
         <v>25</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" ref="D27:D67" si="10">IF(C27&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E27" s="9" t="str">
+      <c r="E27" s="8" t="str">
         <f t="shared" ref="E27:E67" si="11">IF(C27&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <f t="shared" si="9"/>
         <v>26</v>
       </c>
-      <c r="B28" s="15"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D28" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E28" s="9" t="str">
+      <c r="E28" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17">
+      <c r="A29" s="16">
         <f t="shared" si="9"/>
         <v>27</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E29" s="9" t="str">
+      <c r="E29" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <f t="shared" si="9"/>
         <v>28</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E30" s="9" t="str">
+      <c r="E30" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17">
+      <c r="A31" s="16">
         <f t="shared" si="9"/>
         <v>29</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D31" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E31" s="9" t="str">
+      <c r="E31" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16">
+      <c r="A32" s="15">
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E32" s="9" t="str">
+      <c r="E32" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="17">
+      <c r="A33" s="16">
         <f t="shared" si="9"/>
         <v>31</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E33" s="9" t="str">
+      <c r="E33" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
+      <c r="A34" s="15">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="B34" s="15"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E34" s="9" t="str">
+      <c r="E34" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="17">
+      <c r="A35" s="16">
         <f t="shared" si="9"/>
         <v>33</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D35" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E35" s="9" t="str">
+      <c r="E35" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16">
+      <c r="A36" s="15">
         <f t="shared" si="9"/>
         <v>34</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D36" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E36" s="9" t="str">
+      <c r="E36" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17">
+      <c r="A37" s="16">
         <f t="shared" si="9"/>
         <v>35</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D37" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E37" s="9" t="str">
+      <c r="E37" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16">
+      <c r="A38" s="15">
         <f t="shared" si="9"/>
         <v>36</v>
       </c>
-      <c r="B38" s="15"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D38" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E38" s="9" t="str">
+      <c r="E38" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="17">
+      <c r="A39" s="16">
         <f t="shared" si="9"/>
         <v>37</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E39" s="9" t="str">
+      <c r="E39" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16">
+      <c r="A40" s="15">
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
-      <c r="B40" s="15"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D40" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E40" s="9" t="str">
+      <c r="E40" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17">
+      <c r="A41" s="16">
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D41" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E41" s="9" t="str">
+      <c r="E41" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16">
+      <c r="A42" s="15">
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="B42" s="15"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E42" s="9" t="str">
+      <c r="E42" s="8" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>

</xml_diff>

<commit_message>
Adição de Eventos de Interação com o usuário
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="3975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="3975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calendário" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>Testar Modelos e BD</t>
   </si>
@@ -173,12 +173,21 @@
   <si>
     <t>Implementar AD de Grade de horários</t>
   </si>
+  <si>
+    <t>Modelagem do banco</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +214,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,10 +347,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,9 +361,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -336,9 +375,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -368,11 +404,156 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -714,8 +895,8 @@
   </sheetPr>
   <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -728,364 +909,360 @@
     <row r="1" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="4">
+    <row r="4" spans="1:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21">
         <v>42373</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="21">
         <f>B4+1</f>
         <v>42374</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="21">
         <f t="shared" ref="D4:F4" si="0">C4+1</f>
         <v>42375</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="21">
         <f t="shared" si="0"/>
         <v>42376</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="21">
         <f t="shared" si="0"/>
         <v>42377</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="4">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23"/>
+      <c r="B10" s="21">
         <f>F4+3</f>
         <v>42380</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="21">
         <f>B10+1</f>
         <v>42381</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="21">
         <f t="shared" ref="D10:F10" si="1">C10+1</f>
         <v>42382</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="21">
         <f t="shared" si="1"/>
         <v>42383</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="21">
         <f t="shared" si="1"/>
         <v>42384</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4">
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="21">
         <f>F10+3</f>
         <v>42387</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="21">
         <f>B17+1</f>
         <v>42388</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="21">
         <f t="shared" ref="D17:F17" si="2">C17+1</f>
         <v>42389</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="21">
         <f t="shared" si="2"/>
         <v>42390</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="21">
         <f t="shared" si="2"/>
         <v>42391</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8" t="s">
+    <row r="20" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="4">
+    <row r="21" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="2:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="21">
         <f>F17+3</f>
         <v>42394</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="21">
         <f>B24+1</f>
         <v>42395</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="21">
         <f t="shared" ref="D24:F24" si="3">C24+1</f>
         <v>42396</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="21">
         <f t="shared" si="3"/>
         <v>42397</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="21">
         <f t="shared" si="3"/>
         <v>42398</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="8" t="s">
+    <row r="26" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="8" t="s">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="2:6" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1319,10 +1496,10 @@
   <sheetPr codeName="Planilha2">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:I2034"/>
+  <dimension ref="A1:K2034"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1333,755 +1510,765 @@
     <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.25" customWidth="1"/>
+    <col min="11" max="11" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
         <f t="shared" ref="A3" si="0">IF(C3 &lt;&gt; 0,A2+1)</f>
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f>IF(C3&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="str">
-        <f>IF(C3&lt;&gt;"","A","")</f>
-        <v>A</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
+      <c r="K3" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
         <f>IF(C5 &lt;&gt; 0,A3+1)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>IF(C5&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
         <f>IF(C7 &lt;&gt; 0,A4+1)</f>
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f t="shared" ref="D5:D10" si="1">IF(C7&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E5" s="8" t="str">
-        <f t="shared" ref="E5:E12" si="2">IF(C7&lt;&gt;"","A","")</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
         <f>IF(C8 &lt;&gt; 0,A5+1)</f>
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E6" s="8" t="str">
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="26">
+        <f>COUNTIF(E3:E42,"C")/COUNTA(E3:E42)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <f>IF(C9 &lt;&gt; 0,A6+1)</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <f>IF(C10 &lt;&gt; 0,A7+1)</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f t="shared" ref="E5:E12" si="2">IF(C10&lt;&gt;"","A","")</f>
+        <v>A</v>
+      </c>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <f>IF(C11 &lt;&gt; 0,A8+1)</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="7" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
-        <f>IF(C9 &lt;&gt; 0,A6+1)</f>
-        <v>5</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <f>IF(C12 &lt;&gt; 0,A9+1,"")</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E7" s="8" t="str">
+      <c r="E10" s="7" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
-        <f>IF(C10 &lt;&gt; 0,A7+1)</f>
-        <v>6</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="8" t="str">
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <f>IF(C13 &lt;&gt; 0,A10+1,"")</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
-        <f>IF(C11 &lt;&gt; 0,A8+1)</f>
-        <v>7</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="6">
-        <f t="shared" si="1"/>
+    <row r="12" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <f>IF(C14 &lt;&gt; 0,A11+1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <f>IF(C14&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E9" s="8" t="str">
+      <c r="E12" s="7" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
-        <f>IF(C12 &lt;&gt; 0,A9+1,"")</f>
-        <v>8</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E10" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
-        <f>IF(C13 &lt;&gt; 0,A10+1,"")</f>
-        <v>9</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <f>IF(C14 &lt;&gt; 0,A11+1,"")</f>
-        <v>10</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="6">
-        <f>IF(C14&lt;&gt;"",1,"")</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
         <f t="shared" ref="A13:A23" si="3">IF(C14 &lt;&gt; 0,A12+1,"")</f>
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f t="shared" ref="D13:D23" si="4">IF(C14&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E13" s="8" t="str">
+      <c r="E13" s="7" t="str">
         <f t="shared" ref="E13:E23" si="5">IF(C14&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
+    <row r="14" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E14" s="8" t="str">
+      <c r="E14" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+    <row r="15" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E15" s="8" t="str">
+      <c r="E15" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E16" s="8" t="str">
+      <c r="E16" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E17" s="8" t="str">
+      <c r="E17" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E18" s="8" t="str">
+      <c r="E18" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="E19" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15">
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="E20" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E21" s="8" t="str">
+      <c r="E21" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15">
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="E22" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16">
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E23" s="8" t="str">
+      <c r="E23" s="7" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="13">
         <f>IF(C24&lt;&gt; 0,A23+1,"")</f>
         <v>22</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <f>IF(C24&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E24" s="8" t="str">
+      <c r="E24" s="7" t="str">
         <f>IF(C24&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14">
         <f>IF(C25 &lt;&gt; 0,A24+1,"")</f>
         <v>23</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <f>IF(C25&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E25" s="8" t="str">
+      <c r="E25" s="7" t="str">
         <f>IF(C25&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
         <f t="shared" ref="A26" si="6">IF(C26 &lt;&gt; 0,A25+1,"")</f>
         <v>24</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <f t="shared" ref="D26" si="7">IF(C26&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E26" s="8" t="str">
+      <c r="E26" s="7" t="str">
         <f t="shared" ref="E26" si="8">IF(C26&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14">
         <f t="shared" ref="A27:A73" si="9">IF(C27 &lt;&gt; 0,A26+1,"")</f>
         <v>25</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <f t="shared" ref="D27:D67" si="10">IF(C27&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E27" s="8" t="str">
+      <c r="E27" s="7" t="str">
         <f t="shared" ref="E27:E67" si="11">IF(C27&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="15">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
         <f t="shared" si="9"/>
         <v>26</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E28" s="8" t="str">
+      <c r="E28" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14">
         <f t="shared" si="9"/>
         <v>27</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E29" s="8" t="str">
+      <c r="E29" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13">
         <f t="shared" si="9"/>
         <v>28</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E30" s="8" t="str">
+      <c r="E30" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14">
         <f t="shared" si="9"/>
         <v>29</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E31" s="8" t="str">
+      <c r="E31" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="15">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="13">
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="12"/>
+      <c r="C32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E32" s="8" t="str">
+      <c r="E32" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14">
         <f t="shared" si="9"/>
         <v>31</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="12"/>
+      <c r="C33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E33" s="8" t="str">
+      <c r="E33" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13">
         <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="12"/>
+      <c r="C34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E34" s="8" t="str">
+      <c r="E34" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14">
         <f t="shared" si="9"/>
         <v>33</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="12"/>
+      <c r="C35" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E35" s="8" t="str">
+      <c r="E35" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="13">
         <f t="shared" si="9"/>
         <v>34</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="12"/>
+      <c r="C36" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E36" s="8" t="str">
+      <c r="E36" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14">
         <f t="shared" si="9"/>
         <v>35</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="12"/>
+      <c r="C37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E37" s="8" t="str">
+      <c r="E37" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="15">
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="13">
         <f t="shared" si="9"/>
         <v>36</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="6" t="s">
+      <c r="B38" s="12"/>
+      <c r="C38" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E38" s="8" t="str">
+      <c r="E38" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="16">
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14">
         <f t="shared" si="9"/>
         <v>37</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="12"/>
+      <c r="C39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E39" s="8" t="str">
+      <c r="E39" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="15">
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="6" t="s">
+      <c r="B40" s="12"/>
+      <c r="C40" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E40" s="8" t="str">
+      <c r="E40" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="14">
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="12"/>
+      <c r="C41" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E41" s="8" t="str">
+      <c r="E41" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="15">
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="13">
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="12"/>
+      <c r="C42" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E42" s="8" t="str">
+      <c r="E42" s="7" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
@@ -14922,28 +15109,88 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E25 E27:E1011">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{283644A9-E928-417C-A63D-B1E4FE4FBB1A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6 K3">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{34B18192-DD78-4510-827D-55E04E39EF28}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{283644A9-E928-417C-A63D-B1E4FE4FBB1A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{34B18192-DD78-4510-827D-55E04E39EF28}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H6 K3</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
InfraEstrutura: Delete e ajustes
• Impletado Delete
• Ajustes no comportamento da interface
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\C#\Projeto\GradeDeHorario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\C#\GradeDeHorario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="3975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calendário" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Testar Modelos e BD</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>Concluído</t>
+  </si>
+  <si>
+    <t>InfraEs - Delete RN e AD</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Professor - Consultas em RN e AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Professor - Criar consultas Insert, update select e delete</t>
+  </si>
+  <si>
+    <t>Curso - Alterar indent. No Sistema</t>
   </si>
 </sst>
 </file>
@@ -352,7 +367,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,7 +378,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,9 +415,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,133 +438,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -895,8 +801,8 @@
   </sheetPr>
   <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -909,360 +815,320 @@
     <row r="1" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21">
+    <row r="4" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19">
         <v>42373</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <f>B4+1</f>
         <v>42374</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="19">
         <f t="shared" ref="D4:F4" si="0">C4+1</f>
         <v>42375</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <f t="shared" si="0"/>
         <v>42376</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="19">
         <f t="shared" si="0"/>
         <v>42377</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7" t="s">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="21">
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="19">
         <f>F4+3</f>
         <v>42380</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="19">
         <f>B10+1</f>
         <v>42381</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="19">
         <f t="shared" ref="D10:F10" si="1">C10+1</f>
         <v>42382</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <f t="shared" si="1"/>
         <v>42383</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="19">
         <f t="shared" si="1"/>
         <v>42384</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="F11" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="2:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="21">
+      <c r="F12" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19">
         <f>F10+3</f>
         <v>42387</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="19">
         <f>B17+1</f>
         <v>42388</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="19">
         <f t="shared" ref="D17:F17" si="2">C17+1</f>
         <v>42389</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="19">
         <f t="shared" si="2"/>
         <v>42390</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="19">
         <f t="shared" si="2"/>
         <v>42391</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="2:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="21">
+    <row r="18" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="19">
         <f>F17+3</f>
         <v>42394</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="19">
         <f>B24+1</f>
         <v>42395</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="19">
         <f t="shared" ref="D24:F24" si="3">C24+1</f>
         <v>42396</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="19">
         <f t="shared" si="3"/>
         <v>42397</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="19">
         <f t="shared" si="3"/>
         <v>42398</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="2:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+    <row r="25" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:6" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1499,7 +1365,7 @@
   <dimension ref="A1:K2034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C32" sqref="C32:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1517,758 +1383,743 @@
     <row r="1" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
         <f t="shared" ref="A3" si="0">IF(C3 &lt;&gt; 0,A2+1)</f>
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <f>IF(C3&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
         <f>IF(C5 &lt;&gt; 0,A3+1)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <f>IF(C5&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="H4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
         <f>IF(C7 &lt;&gt; 0,A4+1)</f>
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <f t="shared" ref="D5:D10" si="1">IF(C7&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
         <f>IF(C8 &lt;&gt; 0,A5+1)</f>
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="24">
         <f>COUNTIF(E3:E42,"C")/COUNTA(E3:E42)</f>
-        <v>0.1</v>
-      </c>
-      <c r="I6" s="27" t="s">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I6" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
         <f>IF(C9 &lt;&gt; 0,A6+1)</f>
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="24"/>
-    </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
         <f>IF(C10 &lt;&gt; 0,A7+1)</f>
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
+        <f>IF(C11 &lt;&gt; 0,A8+1)</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E8" s="7" t="str">
-        <f t="shared" ref="E5:E12" si="2">IF(C10&lt;&gt;"","A","")</f>
-        <v>A</v>
-      </c>
-      <c r="H8" s="24"/>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
-        <f>IF(C11 &lt;&gt; 0,A8+1)</f>
-        <v>7</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <f>IF(C12 &lt;&gt; 0,A9+1,"")</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="str">
+      <c r="E10" s="6" t="str">
+        <f t="shared" ref="E8:E12" si="2">IF(C12&lt;&gt;"","A","")</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <f>IF(C13 &lt;&gt; 0,A10+1,"")</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <f>IF(C14 &lt;&gt; 0,A11+1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <f>IF(C14&lt;&gt;"",1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
-        <f>IF(C12 &lt;&gt; 0,A9+1,"")</f>
-        <v>8</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E10" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14">
-        <f>IF(C13 &lt;&gt; 0,A10+1,"")</f>
-        <v>9</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2</v>
-      </c>
-      <c r="E11" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
-        <f>IF(C14 &lt;&gt; 0,A11+1,"")</f>
-        <v>10</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5">
-        <f>IF(C14&lt;&gt;"",1,"")</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
         <f t="shared" ref="A13:A23" si="3">IF(C14 &lt;&gt; 0,A12+1,"")</f>
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f t="shared" ref="D13:D23" si="4">IF(C14&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E13" s="7" t="str">
+      <c r="E13" s="6" t="str">
         <f t="shared" ref="E13:E23" si="5">IF(C14&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E14" s="7" t="str">
+      <c r="E14" s="6" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E15" s="7" t="str">
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13">
+    <row r="18" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E16" s="7" t="str">
+      <c r="E18" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+    <row r="20" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12">
         <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E17" s="7" t="str">
+      <c r="E20" s="6" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13">
+    <row r="21" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13">
         <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E18" s="7" t="str">
+      <c r="E21" s="6" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+    <row r="22" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12">
         <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E19" s="7" t="str">
+      <c r="E22" s="6" t="str">
         <f t="shared" si="5"/>
         <v>A</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
+    <row r="23" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
         <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E20" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+      <c r="E23" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12">
         <f>IF(C24&lt;&gt; 0,A23+1,"")</f>
         <v>22</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <f>IF(C24&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E24" s="7" t="str">
+      <c r="E24" s="6" t="str">
         <f>IF(C24&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14">
+    <row r="25" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
         <f>IF(C25 &lt;&gt; 0,A24+1,"")</f>
         <v>23</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <f>IF(C25&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E25" s="7" t="str">
+      <c r="E25" s="6" t="str">
         <f>IF(C25&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
+    <row r="26" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12">
         <f t="shared" ref="A26" si="6">IF(C26 &lt;&gt; 0,A25+1,"")</f>
         <v>24</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <f t="shared" ref="D26" si="7">IF(C26&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E26" s="7" t="str">
+      <c r="E26" s="6" t="str">
         <f t="shared" ref="E26" si="8">IF(C26&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14">
+    <row r="27" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
         <f t="shared" ref="A27:A73" si="9">IF(C27 &lt;&gt; 0,A26+1,"")</f>
         <v>25</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <f t="shared" ref="D27:D67" si="10">IF(C27&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E27" s="7" t="str">
-        <f t="shared" ref="E27:E67" si="11">IF(C27&lt;&gt;"","A","")</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13">
+      <c r="E27" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="12">
         <f t="shared" si="9"/>
         <v>26</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="5" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E28" s="7" t="str">
+      <c r="E28" s="6" t="str">
+        <f t="shared" ref="E27:E67" si="11">IF(C28&lt;&gt;"","A","")</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="12">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14">
+    <row r="31" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13">
         <f t="shared" si="9"/>
-        <v>27</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="5">
+        <v>29</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E29" s="7" t="str">
+      <c r="E31" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="13">
         <f t="shared" si="9"/>
-        <v>28</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="5">
+        <v>31</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E30" s="7" t="str">
+      <c r="E33" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14">
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12">
         <f t="shared" si="9"/>
-        <v>29</v>
-      </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="5">
+        <v>32</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E31" s="7" t="str">
+      <c r="E34" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="13">
+        <f t="shared" si="9"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12">
         <f t="shared" si="9"/>
-        <v>30</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E32" s="7" t="str">
+      <c r="E36" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="13">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="12">
         <f t="shared" si="9"/>
-        <v>31</v>
-      </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E33" s="7" t="str">
+      <c r="E38" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <f t="shared" si="9"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12">
         <f t="shared" si="9"/>
-        <v>32</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="5">
+      <c r="B40" s="11"/>
+      <c r="C40" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E34" s="7" t="str">
+      <c r="E40" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14">
+    <row r="41" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13">
         <f t="shared" si="9"/>
-        <v>33</v>
-      </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="5">
+        <v>39</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E35" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13">
+      <c r="E41" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="12">
         <f t="shared" si="9"/>
-        <v>34</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="5">
+        <v>40</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E36" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14">
-        <f t="shared" si="9"/>
-        <v>35</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E37" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13">
-        <f t="shared" si="9"/>
-        <v>36</v>
-      </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E38" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14">
-        <f t="shared" si="9"/>
-        <v>37</v>
-      </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13">
-        <f t="shared" si="9"/>
-        <v>38</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E40" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14">
-        <f t="shared" si="9"/>
-        <v>39</v>
-      </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13">
-        <f t="shared" si="9"/>
-        <v>40</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="7" t="str">
+      <c r="E42" s="6" t="str">
         <f t="shared" si="11"/>
         <v>A</v>
       </c>

</xml_diff>

<commit_message>
Infraestrutura e Professor: Melhoras na codificação
Interface, RN e AD
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>Testar Modelos e BD</t>
   </si>
@@ -438,9 +438,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -451,6 +448,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -935,7 +935,7 @@
       <c r="E11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="29" t="s">
         <v>51</v>
       </c>
     </row>
@@ -952,7 +952,7 @@
       <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="28" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
   <dimension ref="A1:K2034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:E33"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1384,10 +1384,10 @@
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="9" t="s">
         <v>31</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="4">
@@ -1433,7 +1433,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="4">
@@ -1456,7 +1456,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4">
@@ -1473,7 +1473,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="H6" s="24">
         <f>COUNTIF(E3:E42,"C")/COUNTA(E3:E42)</f>
-        <v>0.47499999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>50</v>
@@ -1497,7 +1497,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="4">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4">
@@ -1532,7 +1532,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4">
@@ -1549,16 +1549,15 @@
         <v>8</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E10" s="6" t="str">
-        <f t="shared" ref="E8:E12" si="2">IF(C12&lt;&gt;"","A","")</f>
-        <v>A</v>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1567,7 +1566,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4">
@@ -1583,7 +1582,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4">
@@ -1591,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E10:E12" si="2">IF(C14&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
@@ -1601,7 +1600,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4">
@@ -1609,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f t="shared" ref="E13:E23" si="5">IF(C14&lt;&gt;"","A","")</f>
+        <f t="shared" ref="E13:E22" si="5">IF(C14&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
@@ -1619,7 +1618,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="4">
@@ -1637,7 +1636,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="4">
@@ -1654,7 +1653,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4">
@@ -1671,16 +1670,15 @@
         <v>15</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E17" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
+      <c r="E17" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1689,7 +1687,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="4">
@@ -1706,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="4">
@@ -1724,7 +1722,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="4">
@@ -1742,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="4">
@@ -1760,7 +1758,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="4">
@@ -1778,7 +1776,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="11"/>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="4">
@@ -1795,16 +1793,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="4">
         <f>IF(C24&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
-      <c r="E24" s="6" t="str">
-        <f>IF(C24&lt;&gt;"","A","")</f>
-        <v>A</v>
+      <c r="E24" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1813,7 +1810,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="4">
@@ -1831,7 +1828,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="11"/>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="4">
@@ -1849,7 +1846,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="11"/>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>32</v>
       </c>
       <c r="D27" s="4">
@@ -1866,7 +1863,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D28" s="4">
@@ -1874,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f t="shared" ref="E27:E67" si="11">IF(C28&lt;&gt;"","A","")</f>
+        <f t="shared" ref="E28:E67" si="11">IF(C28&lt;&gt;"","A","")</f>
         <v>A</v>
       </c>
     </row>
@@ -1884,7 +1881,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="4">
@@ -1901,16 +1898,15 @@
         <v>28</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E30" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
+      <c r="E30" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1919,7 +1915,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="11"/>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="27" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="4">
@@ -1927,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1936,7 +1932,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="11"/>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="4">
@@ -1954,7 +1950,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="4">
@@ -1972,7 +1968,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="4">
@@ -1989,7 +1985,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="27" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="4">
@@ -2007,7 +2003,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="27" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="4">
@@ -2024,16 +2020,15 @@
         <v>35</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="27" t="s">
         <v>40</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="E37" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v>A</v>
+      <c r="E37" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2042,7 +2037,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="11"/>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="27" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="4">
@@ -2059,7 +2054,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="27" t="s">
         <v>42</v>
       </c>
       <c r="D39" s="4">
@@ -2077,7 +2072,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>43</v>
       </c>
       <c r="D40" s="4">
@@ -2095,7 +2090,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="27" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="4">
@@ -2112,7 +2107,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D42" s="4">

</xml_diff>